<commit_message>
Added Enviroment.txt, updated readme file and included current image with the issue.
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -1,50 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raza\Desktop\Python\StockAnalysis\PythonExcelPowerBIRefresh\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2620A439-E635-4CCE-A5CA-D7ACFB897880}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7545" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Raza</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>Zohair</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -60,15 +65,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -356,20 +370,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,17 +391,17 @@
       </c>
       <c r="D1">
         <f>VLOOKUP(C1,A$1:B$2,2,0)+3</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1">
         <f>B1+1</f>
-        <v/>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -403,17 +413,17 @@
       </c>
       <c r="D2">
         <f>VLOOKUP(C2,A$1:B$2,2,0)+3</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2">
         <f>B2+1</f>
-        <v/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>